<commit_message>
Starting Basic UI Design
</commit_message>
<xml_diff>
--- a/Doc/FootballTaggingProject_CurrentWorkflow.xlsx
+++ b/Doc/FootballTaggingProject_CurrentWorkflow.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yingy\Desktop\FootballTaggingProject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yingy\Desktop\FootballTaggingProject\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{712C8CD1-207F-4893-9A37-1A00CDDDD6EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62BCC092-5530-4330-B06F-B998A27C1156}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3270" yWindow="3255" windowWidth="20820" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="825" yWindow="-120" windowWidth="28095" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -321,7 +321,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -340,6 +340,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="13">
     <border>
@@ -519,9 +525,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -542,6 +547,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="45" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="45" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="45" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -551,9 +559,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="45" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="45" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -836,446 +843,446 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17" style="24" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.140625" style="24" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" style="24" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16" style="24" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="9.140625" style="2"/>
-    <col min="7" max="9" width="11.7109375" style="2" customWidth="1"/>
-    <col min="10" max="10" width="14.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17" style="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" style="20" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16" style="20" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="9.140625" style="1"/>
+    <col min="7" max="9" width="11.7109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="14.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="23" t="s">
+      <c r="C1" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="23" t="s">
+      <c r="D1" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="E1" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="F1" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="G1" s="17" t="s">
+      <c r="G1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="H1" s="17" t="s">
+      <c r="H1" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="17" t="s">
+      <c r="I1" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="17" t="s">
+      <c r="J1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="K1" s="17" t="s">
+      <c r="K1" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="L1" s="17" t="s">
+      <c r="L1" s="16" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="C2" s="25" t="s">
+      <c r="C2" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="D2" s="25" t="s">
+      <c r="D2" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="1">
         <v>0</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2" s="1">
         <v>1</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="J2" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="K2" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="L2" s="1" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="B3" s="25" t="s">
+      <c r="B3" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="C3" s="25" t="s">
+      <c r="C3" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="D3" s="25" t="s">
+      <c r="D3" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="1">
         <v>0</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="1">
         <v>1</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="H3" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="I3" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="J3" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="K3" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="L3" s="2" t="s">
+      <c r="L3" s="1" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="25" t="s">
+      <c r="A4" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="B4" s="25" t="s">
+      <c r="B4" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="C4" s="25" t="s">
+      <c r="C4" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="D4" s="25" t="s">
+      <c r="D4" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="1">
         <v>0</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="1">
         <v>1</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G4" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="H4" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="I4" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="J4" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="K4" s="2" t="s">
+      <c r="K4" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="L4" s="2" t="s">
+      <c r="L4" s="1" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="25" t="s">
+      <c r="A5" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="B5" s="25" t="s">
+      <c r="B5" s="21" t="s">
         <v>84</v>
       </c>
-      <c r="C5" s="25" t="s">
+      <c r="C5" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="D5" s="25" t="s">
+      <c r="D5" s="21" t="s">
         <v>83</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="1">
         <v>0</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5" s="1">
         <v>1</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="G5" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="H5" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="I5" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="J5" s="2" t="s">
+      <c r="J5" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="K5" s="2" t="s">
+      <c r="K5" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="L5" s="2" t="s">
+      <c r="L5" s="1" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="25"/>
-      <c r="B6" s="25"/>
-      <c r="C6" s="25"/>
-      <c r="D6" s="25"/>
+      <c r="A6" s="21"/>
+      <c r="B6" s="21"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="21"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="25"/>
-      <c r="B7" s="25"/>
-      <c r="C7" s="25"/>
-      <c r="D7" s="25"/>
+      <c r="A7" s="21"/>
+      <c r="B7" s="21"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="21"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="25"/>
-      <c r="B8" s="25"/>
-      <c r="C8" s="25"/>
-      <c r="D8" s="25"/>
+      <c r="A8" s="21"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="21"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="25"/>
-      <c r="B9" s="25"/>
-      <c r="C9" s="25"/>
-      <c r="D9" s="25"/>
+      <c r="A9" s="21"/>
+      <c r="B9" s="21"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="21"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="25"/>
-      <c r="B10" s="25"/>
-      <c r="C10" s="25"/>
-      <c r="D10" s="25"/>
+      <c r="A10" s="21"/>
+      <c r="B10" s="21"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="21"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="25"/>
-      <c r="B11" s="25"/>
-      <c r="C11" s="25"/>
-      <c r="D11" s="25"/>
+      <c r="A11" s="21"/>
+      <c r="B11" s="21"/>
+      <c r="C11" s="21"/>
+      <c r="D11" s="21"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="25"/>
-      <c r="B12" s="25"/>
-      <c r="C12" s="25"/>
-      <c r="D12" s="25"/>
+      <c r="A12" s="21"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="21"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="25"/>
-      <c r="B13" s="25"/>
-      <c r="C13" s="25"/>
-      <c r="D13" s="25"/>
+      <c r="A13" s="21"/>
+      <c r="B13" s="21"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="21"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="25"/>
-      <c r="B14" s="25"/>
-      <c r="C14" s="25"/>
-      <c r="D14" s="25"/>
+      <c r="A14" s="21"/>
+      <c r="B14" s="21"/>
+      <c r="C14" s="21"/>
+      <c r="D14" s="21"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="25"/>
-      <c r="B15" s="25"/>
-      <c r="C15" s="25"/>
-      <c r="D15" s="25"/>
+      <c r="A15" s="21"/>
+      <c r="B15" s="21"/>
+      <c r="C15" s="21"/>
+      <c r="D15" s="21"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="25"/>
-      <c r="B16" s="25"/>
-      <c r="C16" s="25"/>
-      <c r="D16" s="25"/>
+      <c r="A16" s="21"/>
+      <c r="B16" s="21"/>
+      <c r="C16" s="21"/>
+      <c r="D16" s="21"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="25"/>
-      <c r="B17" s="25"/>
-      <c r="C17" s="25"/>
-      <c r="D17" s="25"/>
+      <c r="A17" s="21"/>
+      <c r="B17" s="21"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="21"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="25"/>
-      <c r="B18" s="25"/>
-      <c r="C18" s="25"/>
-      <c r="D18" s="25"/>
+      <c r="A18" s="21"/>
+      <c r="B18" s="21"/>
+      <c r="C18" s="21"/>
+      <c r="D18" s="21"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="25"/>
-      <c r="B19" s="25"/>
-      <c r="C19" s="25"/>
-      <c r="D19" s="25"/>
+      <c r="A19" s="21"/>
+      <c r="B19" s="21"/>
+      <c r="C19" s="21"/>
+      <c r="D19" s="21"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="25"/>
-      <c r="B20" s="25"/>
-      <c r="C20" s="25"/>
-      <c r="D20" s="25"/>
+      <c r="A20" s="21"/>
+      <c r="B20" s="21"/>
+      <c r="C20" s="21"/>
+      <c r="D20" s="21"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="25"/>
-      <c r="B21" s="25"/>
-      <c r="C21" s="25"/>
-      <c r="D21" s="25"/>
+      <c r="A21" s="21"/>
+      <c r="B21" s="21"/>
+      <c r="C21" s="21"/>
+      <c r="D21" s="21"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="25"/>
-      <c r="B22" s="25"/>
-      <c r="C22" s="25"/>
-      <c r="D22" s="25"/>
+      <c r="A22" s="21"/>
+      <c r="B22" s="21"/>
+      <c r="C22" s="21"/>
+      <c r="D22" s="21"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="25"/>
-      <c r="B23" s="25"/>
-      <c r="C23" s="25"/>
-      <c r="D23" s="25"/>
+      <c r="A23" s="21"/>
+      <c r="B23" s="21"/>
+      <c r="C23" s="21"/>
+      <c r="D23" s="21"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="25"/>
-      <c r="B24" s="25"/>
-      <c r="C24" s="25"/>
-      <c r="D24" s="25"/>
+      <c r="A24" s="21"/>
+      <c r="B24" s="21"/>
+      <c r="C24" s="21"/>
+      <c r="D24" s="21"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="25"/>
-      <c r="B25" s="25"/>
-      <c r="C25" s="25"/>
-      <c r="D25" s="25"/>
+      <c r="A25" s="21"/>
+      <c r="B25" s="21"/>
+      <c r="C25" s="21"/>
+      <c r="D25" s="21"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="25"/>
-      <c r="B26" s="25"/>
-      <c r="C26" s="25"/>
-      <c r="D26" s="25"/>
+      <c r="A26" s="21"/>
+      <c r="B26" s="21"/>
+      <c r="C26" s="21"/>
+      <c r="D26" s="21"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="25"/>
-      <c r="B27" s="25"/>
-      <c r="C27" s="25"/>
-      <c r="D27" s="25"/>
+      <c r="A27" s="21"/>
+      <c r="B27" s="21"/>
+      <c r="C27" s="21"/>
+      <c r="D27" s="21"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="25"/>
-      <c r="B28" s="25"/>
-      <c r="C28" s="25"/>
-      <c r="D28" s="25"/>
+      <c r="A28" s="21"/>
+      <c r="B28" s="21"/>
+      <c r="C28" s="21"/>
+      <c r="D28" s="21"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="25"/>
-      <c r="B29" s="25"/>
-      <c r="C29" s="25"/>
-      <c r="D29" s="25"/>
+      <c r="A29" s="21"/>
+      <c r="B29" s="21"/>
+      <c r="C29" s="21"/>
+      <c r="D29" s="21"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="25"/>
-      <c r="B30" s="25"/>
-      <c r="C30" s="25"/>
-      <c r="D30" s="25"/>
+      <c r="A30" s="21"/>
+      <c r="B30" s="21"/>
+      <c r="C30" s="21"/>
+      <c r="D30" s="21"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="25"/>
-      <c r="B31" s="25"/>
-      <c r="C31" s="25"/>
-      <c r="D31" s="25"/>
+      <c r="A31" s="21"/>
+      <c r="B31" s="21"/>
+      <c r="C31" s="21"/>
+      <c r="D31" s="21"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="25"/>
-      <c r="B32" s="25"/>
-      <c r="C32" s="25"/>
-      <c r="D32" s="25"/>
+      <c r="A32" s="21"/>
+      <c r="B32" s="21"/>
+      <c r="C32" s="21"/>
+      <c r="D32" s="21"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="25"/>
-      <c r="B33" s="25"/>
-      <c r="C33" s="25"/>
-      <c r="D33" s="25"/>
+      <c r="A33" s="21"/>
+      <c r="B33" s="21"/>
+      <c r="C33" s="21"/>
+      <c r="D33" s="21"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="25"/>
-      <c r="B34" s="25"/>
-      <c r="C34" s="25"/>
-      <c r="D34" s="25"/>
+      <c r="A34" s="21"/>
+      <c r="B34" s="21"/>
+      <c r="C34" s="21"/>
+      <c r="D34" s="21"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="25"/>
-      <c r="B35" s="25"/>
-      <c r="C35" s="25"/>
-      <c r="D35" s="25"/>
+      <c r="A35" s="21"/>
+      <c r="B35" s="21"/>
+      <c r="C35" s="21"/>
+      <c r="D35" s="21"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="25"/>
-      <c r="B36" s="25"/>
-      <c r="C36" s="25"/>
-      <c r="D36" s="25"/>
+      <c r="A36" s="21"/>
+      <c r="B36" s="21"/>
+      <c r="C36" s="21"/>
+      <c r="D36" s="21"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="25"/>
-      <c r="B37" s="25"/>
-      <c r="C37" s="25"/>
-      <c r="D37" s="25"/>
+      <c r="A37" s="21"/>
+      <c r="B37" s="21"/>
+      <c r="C37" s="21"/>
+      <c r="D37" s="21"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="25"/>
-      <c r="B38" s="25"/>
-      <c r="C38" s="25"/>
-      <c r="D38" s="25"/>
+      <c r="A38" s="21"/>
+      <c r="B38" s="21"/>
+      <c r="C38" s="21"/>
+      <c r="D38" s="21"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="25"/>
-      <c r="B39" s="25"/>
-      <c r="C39" s="25"/>
-      <c r="D39" s="25"/>
+      <c r="A39" s="21"/>
+      <c r="B39" s="21"/>
+      <c r="C39" s="21"/>
+      <c r="D39" s="21"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="25"/>
-      <c r="B40" s="25"/>
-      <c r="C40" s="25"/>
-      <c r="D40" s="25"/>
+      <c r="A40" s="21"/>
+      <c r="B40" s="21"/>
+      <c r="C40" s="21"/>
+      <c r="D40" s="21"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="25"/>
-      <c r="B41" s="25"/>
-      <c r="C41" s="25"/>
-      <c r="D41" s="25"/>
+      <c r="A41" s="21"/>
+      <c r="B41" s="21"/>
+      <c r="C41" s="21"/>
+      <c r="D41" s="21"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="25"/>
-      <c r="B42" s="25"/>
-      <c r="C42" s="25"/>
-      <c r="D42" s="25"/>
+      <c r="A42" s="21"/>
+      <c r="B42" s="21"/>
+      <c r="C42" s="21"/>
+      <c r="D42" s="21"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="25"/>
-      <c r="B43" s="25"/>
-      <c r="C43" s="25"/>
-      <c r="D43" s="25"/>
+      <c r="A43" s="21"/>
+      <c r="B43" s="21"/>
+      <c r="C43" s="21"/>
+      <c r="D43" s="21"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="25"/>
-      <c r="B44" s="25"/>
-      <c r="C44" s="25"/>
-      <c r="D44" s="25"/>
+      <c r="A44" s="21"/>
+      <c r="B44" s="21"/>
+      <c r="C44" s="21"/>
+      <c r="D44" s="21"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1302,468 +1309,483 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AFE8A7E-74D2-4E50-8D0C-C7B7F22ED1C4}">
-  <dimension ref="B1:AB18"/>
+  <dimension ref="B1:AA18"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="P18" sqref="F18:P18"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4:AA18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="5" width="5.7109375" customWidth="1"/>
+    <col min="4" max="4" width="5.7109375" customWidth="1"/>
+    <col min="5" max="5" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="26" width="3.7109375" customWidth="1"/>
+    <col min="27" max="27" width="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F4" s="20" t="s">
+    <row r="3" spans="2:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="2:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E4" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="F4" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
-      <c r="J4" s="20"/>
-      <c r="K4" s="20"/>
-      <c r="L4" s="21"/>
-      <c r="M4" s="22" t="s">
+      <c r="G4" s="22"/>
+      <c r="H4" s="22"/>
+      <c r="I4" s="22"/>
+      <c r="J4" s="22"/>
+      <c r="K4" s="22"/>
+      <c r="L4" s="23"/>
+      <c r="M4" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="N4" s="20"/>
-      <c r="O4" s="20"/>
-      <c r="P4" s="20"/>
-      <c r="Q4" s="20"/>
-      <c r="R4" s="20"/>
-      <c r="S4" s="21"/>
-      <c r="T4" s="20" t="s">
+      <c r="N4" s="22"/>
+      <c r="O4" s="22"/>
+      <c r="P4" s="22"/>
+      <c r="Q4" s="22"/>
+      <c r="R4" s="22"/>
+      <c r="S4" s="23"/>
+      <c r="T4" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="U4" s="20"/>
-      <c r="V4" s="20"/>
-      <c r="W4" s="20"/>
-      <c r="X4" s="20"/>
-      <c r="Y4" s="20"/>
-      <c r="Z4" s="20"/>
-      <c r="AA4" s="1" t="s">
+      <c r="U4" s="22"/>
+      <c r="V4" s="22"/>
+      <c r="W4" s="22"/>
+      <c r="X4" s="22"/>
+      <c r="Y4" s="22"/>
+      <c r="Z4" s="22"/>
+      <c r="AA4" s="26" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="2:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E5">
-        <v>5</v>
-      </c>
-      <c r="F5" s="3"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
-      <c r="M5" s="4"/>
-      <c r="N5" s="4"/>
-      <c r="O5" s="4"/>
-      <c r="P5" s="4"/>
-      <c r="Q5" s="4"/>
-      <c r="R5" s="4"/>
-      <c r="S5" s="4"/>
-      <c r="T5" s="4"/>
-      <c r="U5" s="4"/>
-      <c r="V5" s="4"/>
-      <c r="W5" s="4"/>
-      <c r="X5" s="4"/>
-      <c r="Y5" s="4"/>
-      <c r="Z5" s="5"/>
-    </row>
-    <row r="6" spans="2:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E6">
-        <v>5</v>
-      </c>
-      <c r="F6" s="6"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
-      <c r="M6" s="2"/>
-      <c r="N6" s="2"/>
-      <c r="O6" s="2"/>
-      <c r="P6" s="2"/>
-      <c r="Q6" s="2"/>
-      <c r="R6" s="2"/>
-      <c r="S6" s="2"/>
-      <c r="T6" s="2"/>
-      <c r="U6" s="2"/>
-      <c r="V6" s="2"/>
-      <c r="W6" s="2"/>
-      <c r="X6" s="2"/>
-      <c r="Y6" s="2"/>
-      <c r="Z6" s="7"/>
-    </row>
-    <row r="7" spans="2:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E7">
-        <v>5</v>
-      </c>
-      <c r="F7" s="6"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
-      <c r="N7" s="2"/>
-      <c r="O7" s="2"/>
-      <c r="P7" s="2"/>
-      <c r="Q7" s="2"/>
-      <c r="R7" s="2"/>
-      <c r="S7" s="2"/>
-      <c r="T7" s="2"/>
-      <c r="U7" s="2"/>
-      <c r="V7" s="2"/>
-      <c r="W7" s="2"/>
-      <c r="X7" s="2"/>
-      <c r="Y7" s="2"/>
-      <c r="Z7" s="7"/>
-    </row>
-    <row r="8" spans="2:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E8">
-        <v>5</v>
-      </c>
-      <c r="F8" s="11"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
-      <c r="M8" s="2"/>
-      <c r="N8" s="2"/>
-      <c r="O8" s="2"/>
-      <c r="P8" s="2"/>
-      <c r="Q8" s="2"/>
-      <c r="R8" s="2"/>
-      <c r="S8" s="2"/>
-      <c r="T8" s="2"/>
-      <c r="U8" s="2"/>
-      <c r="V8" s="2"/>
-      <c r="W8" s="2"/>
-      <c r="X8" s="12"/>
-      <c r="Y8" s="12"/>
-      <c r="Z8" s="13"/>
-    </row>
-    <row r="9" spans="2:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E9">
-        <v>5</v>
-      </c>
-      <c r="F9" s="11"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
-      <c r="L9" s="2"/>
-      <c r="M9" s="2"/>
-      <c r="N9" s="2"/>
-      <c r="O9" s="2"/>
-      <c r="P9" s="2"/>
-      <c r="Q9" s="2"/>
-      <c r="R9" s="2"/>
-      <c r="S9" s="2"/>
-      <c r="T9" s="2"/>
-      <c r="U9" s="2"/>
-      <c r="V9" s="2"/>
-      <c r="W9" s="2"/>
-      <c r="X9" s="12"/>
-      <c r="Y9" s="12"/>
-      <c r="Z9" s="13"/>
-    </row>
-    <row r="10" spans="2:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E10">
-        <v>5</v>
-      </c>
-      <c r="F10" s="14"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
-      <c r="M10" s="2"/>
-      <c r="N10" s="2"/>
-      <c r="O10" s="2"/>
-      <c r="P10" s="2"/>
-      <c r="Q10" s="2"/>
-      <c r="R10" s="2"/>
-      <c r="S10" s="2"/>
-      <c r="T10" s="2"/>
-      <c r="U10" s="2"/>
-      <c r="V10" s="2"/>
-      <c r="W10" s="2"/>
-      <c r="X10" s="12"/>
-      <c r="Y10" s="12"/>
-      <c r="Z10" s="15"/>
-    </row>
-    <row r="11" spans="2:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D11" t="s">
-        <v>46</v>
-      </c>
-      <c r="E11">
-        <v>5</v>
-      </c>
-      <c r="F11" s="14"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
-      <c r="L11" s="2"/>
-      <c r="M11" s="2"/>
-      <c r="N11" s="2"/>
-      <c r="O11" s="2"/>
-      <c r="P11" s="16" t="s">
+    <row r="5" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E5" s="25">
+        <v>5</v>
+      </c>
+      <c r="F5" s="2"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="3"/>
+      <c r="Q5" s="3"/>
+      <c r="R5" s="3"/>
+      <c r="S5" s="3"/>
+      <c r="T5" s="3"/>
+      <c r="U5" s="3"/>
+      <c r="V5" s="3"/>
+      <c r="W5" s="3"/>
+      <c r="X5" s="3"/>
+      <c r="Y5" s="3"/>
+      <c r="Z5" s="4"/>
+      <c r="AA5" s="25"/>
+    </row>
+    <row r="6" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E6" s="25">
+        <v>5</v>
+      </c>
+      <c r="F6" s="5"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1"/>
+      <c r="R6" s="1"/>
+      <c r="S6" s="1"/>
+      <c r="T6" s="1"/>
+      <c r="U6" s="1"/>
+      <c r="V6" s="1"/>
+      <c r="W6" s="1"/>
+      <c r="X6" s="1"/>
+      <c r="Y6" s="1"/>
+      <c r="Z6" s="6"/>
+      <c r="AA6" s="25"/>
+    </row>
+    <row r="7" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E7" s="25">
+        <v>5</v>
+      </c>
+      <c r="F7" s="5"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1"/>
+      <c r="R7" s="1"/>
+      <c r="S7" s="1"/>
+      <c r="T7" s="1"/>
+      <c r="U7" s="1"/>
+      <c r="V7" s="1"/>
+      <c r="W7" s="1"/>
+      <c r="X7" s="1"/>
+      <c r="Y7" s="1"/>
+      <c r="Z7" s="6"/>
+      <c r="AA7" s="25"/>
+    </row>
+    <row r="8" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E8" s="25">
+        <v>5</v>
+      </c>
+      <c r="F8" s="10"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
+      <c r="R8" s="1"/>
+      <c r="S8" s="1"/>
+      <c r="T8" s="1"/>
+      <c r="U8" s="1"/>
+      <c r="V8" s="1"/>
+      <c r="W8" s="1"/>
+      <c r="X8" s="11"/>
+      <c r="Y8" s="11"/>
+      <c r="Z8" s="12"/>
+      <c r="AA8" s="25"/>
+    </row>
+    <row r="9" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E9" s="25">
+        <v>5</v>
+      </c>
+      <c r="F9" s="10"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
+      <c r="Q9" s="1"/>
+      <c r="R9" s="1"/>
+      <c r="S9" s="1"/>
+      <c r="T9" s="1"/>
+      <c r="U9" s="1"/>
+      <c r="V9" s="1"/>
+      <c r="W9" s="1"/>
+      <c r="X9" s="11"/>
+      <c r="Y9" s="11"/>
+      <c r="Z9" s="12"/>
+      <c r="AA9" s="25"/>
+    </row>
+    <row r="10" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E10" s="25">
+        <v>5</v>
+      </c>
+      <c r="F10" s="13"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
+      <c r="Q10" s="1"/>
+      <c r="R10" s="1"/>
+      <c r="S10" s="1"/>
+      <c r="T10" s="1"/>
+      <c r="U10" s="1"/>
+      <c r="V10" s="1"/>
+      <c r="W10" s="1"/>
+      <c r="X10" s="11"/>
+      <c r="Y10" s="11"/>
+      <c r="Z10" s="14"/>
+      <c r="AA10" s="25"/>
+    </row>
+    <row r="11" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E11" s="25">
+        <v>5</v>
+      </c>
+      <c r="F11" s="13"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="Q11" s="2"/>
-      <c r="R11" s="2"/>
-      <c r="S11" s="2"/>
-      <c r="T11" s="2"/>
-      <c r="U11" s="2"/>
-      <c r="V11" s="2"/>
-      <c r="W11" s="2"/>
-      <c r="X11" s="12"/>
-      <c r="Y11" s="12"/>
-      <c r="Z11" s="15"/>
-      <c r="AB11" t="s">
+      <c r="Q11" s="1"/>
+      <c r="R11" s="1"/>
+      <c r="S11" s="1"/>
+      <c r="T11" s="1"/>
+      <c r="U11" s="1"/>
+      <c r="V11" s="1"/>
+      <c r="W11" s="1"/>
+      <c r="X11" s="11"/>
+      <c r="Y11" s="11"/>
+      <c r="Z11" s="14"/>
+      <c r="AA11" s="25"/>
+    </row>
+    <row r="12" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E12" s="25">
+        <v>5</v>
+      </c>
+      <c r="F12" s="13"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
+      <c r="Q12" s="1"/>
+      <c r="R12" s="1"/>
+      <c r="S12" s="1"/>
+      <c r="T12" s="1"/>
+      <c r="U12" s="1"/>
+      <c r="V12" s="1"/>
+      <c r="W12" s="1"/>
+      <c r="X12" s="11"/>
+      <c r="Y12" s="11"/>
+      <c r="Z12" s="14"/>
+      <c r="AA12" s="25"/>
+    </row>
+    <row r="13" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E13" s="25">
+        <v>5</v>
+      </c>
+      <c r="F13" s="10"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
+      <c r="Q13" s="1"/>
+      <c r="R13" s="1"/>
+      <c r="S13" s="1"/>
+      <c r="T13" s="1"/>
+      <c r="U13" s="1"/>
+      <c r="V13" s="1"/>
+      <c r="W13" s="1"/>
+      <c r="X13" s="11"/>
+      <c r="Y13" s="11"/>
+      <c r="Z13" s="12"/>
+      <c r="AA13" s="25"/>
+    </row>
+    <row r="14" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E14" s="25">
+        <v>5</v>
+      </c>
+      <c r="F14" s="10"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+      <c r="P14" s="1"/>
+      <c r="Q14" s="1"/>
+      <c r="R14" s="1"/>
+      <c r="S14" s="1"/>
+      <c r="T14" s="1"/>
+      <c r="U14" s="1"/>
+      <c r="V14" s="1"/>
+      <c r="W14" s="1"/>
+      <c r="X14" s="11"/>
+      <c r="Y14" s="11"/>
+      <c r="Z14" s="12"/>
+      <c r="AA14" s="25"/>
+    </row>
+    <row r="15" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E15" s="25">
+        <v>5</v>
+      </c>
+      <c r="F15" s="5"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="1"/>
+      <c r="Q15" s="1"/>
+      <c r="R15" s="1"/>
+      <c r="S15" s="1"/>
+      <c r="T15" s="1"/>
+      <c r="U15" s="1"/>
+      <c r="V15" s="1"/>
+      <c r="W15" s="1"/>
+      <c r="X15" s="1"/>
+      <c r="Y15" s="1"/>
+      <c r="Z15" s="6"/>
+      <c r="AA15" s="25"/>
+    </row>
+    <row r="16" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E16" s="25">
+        <v>5</v>
+      </c>
+      <c r="F16" s="5"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+      <c r="P16" s="1"/>
+      <c r="Q16" s="1"/>
+      <c r="R16" s="1"/>
+      <c r="S16" s="1"/>
+      <c r="T16" s="1"/>
+      <c r="U16" s="1"/>
+      <c r="V16" s="1"/>
+      <c r="W16" s="1"/>
+      <c r="X16" s="1"/>
+      <c r="Y16" s="1"/>
+      <c r="Z16" s="6"/>
+      <c r="AA16" s="25"/>
+    </row>
+    <row r="17" spans="5:27" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E17" s="25">
+        <v>5</v>
+      </c>
+      <c r="F17" s="7"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="8"/>
+      <c r="K17" s="8"/>
+      <c r="L17" s="8"/>
+      <c r="M17" s="8"/>
+      <c r="N17" s="8"/>
+      <c r="O17" s="8"/>
+      <c r="P17" s="8"/>
+      <c r="Q17" s="8"/>
+      <c r="R17" s="8"/>
+      <c r="S17" s="8"/>
+      <c r="T17" s="8"/>
+      <c r="U17" s="8"/>
+      <c r="V17" s="8"/>
+      <c r="W17" s="8"/>
+      <c r="X17" s="8"/>
+      <c r="Y17" s="8"/>
+      <c r="Z17" s="9"/>
+      <c r="AA17" s="25"/>
+    </row>
+    <row r="18" spans="5:27" x14ac:dyDescent="0.25">
+      <c r="E18" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="F18" s="25">
+        <v>5</v>
+      </c>
+      <c r="G18" s="25">
+        <v>5</v>
+      </c>
+      <c r="H18" s="25">
+        <v>5</v>
+      </c>
+      <c r="I18" s="25">
+        <v>5</v>
+      </c>
+      <c r="J18" s="25">
+        <v>5</v>
+      </c>
+      <c r="K18" s="25">
+        <v>5</v>
+      </c>
+      <c r="L18" s="25">
+        <v>5</v>
+      </c>
+      <c r="M18" s="25">
+        <v>5</v>
+      </c>
+      <c r="N18" s="25">
+        <v>5</v>
+      </c>
+      <c r="O18" s="25">
+        <v>5</v>
+      </c>
+      <c r="P18" s="25">
+        <v>5</v>
+      </c>
+      <c r="Q18" s="25">
+        <v>5</v>
+      </c>
+      <c r="R18" s="25">
+        <v>5</v>
+      </c>
+      <c r="S18" s="25">
+        <v>5</v>
+      </c>
+      <c r="T18" s="25">
+        <v>5</v>
+      </c>
+      <c r="U18" s="25">
+        <v>5</v>
+      </c>
+      <c r="V18" s="25">
+        <v>5</v>
+      </c>
+      <c r="W18" s="25">
+        <v>5</v>
+      </c>
+      <c r="X18" s="25">
+        <v>5</v>
+      </c>
+      <c r="Y18" s="25">
+        <v>5</v>
+      </c>
+      <c r="Z18" s="25">
+        <v>5</v>
+      </c>
+      <c r="AA18" s="25" t="s">
         <v>47</v>
-      </c>
-    </row>
-    <row r="12" spans="2:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E12">
-        <v>5</v>
-      </c>
-      <c r="F12" s="14"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
-      <c r="L12" s="2"/>
-      <c r="M12" s="2"/>
-      <c r="N12" s="2"/>
-      <c r="O12" s="2"/>
-      <c r="P12" s="2"/>
-      <c r="Q12" s="2"/>
-      <c r="R12" s="2"/>
-      <c r="S12" s="2"/>
-      <c r="T12" s="2"/>
-      <c r="U12" s="2"/>
-      <c r="V12" s="2"/>
-      <c r="W12" s="2"/>
-      <c r="X12" s="12"/>
-      <c r="Y12" s="12"/>
-      <c r="Z12" s="15"/>
-    </row>
-    <row r="13" spans="2:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E13">
-        <v>5</v>
-      </c>
-      <c r="F13" s="11"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
-      <c r="K13" s="2"/>
-      <c r="L13" s="2"/>
-      <c r="M13" s="2"/>
-      <c r="N13" s="2"/>
-      <c r="O13" s="2"/>
-      <c r="P13" s="2"/>
-      <c r="Q13" s="2"/>
-      <c r="R13" s="2"/>
-      <c r="S13" s="2"/>
-      <c r="T13" s="2"/>
-      <c r="U13" s="2"/>
-      <c r="V13" s="2"/>
-      <c r="W13" s="2"/>
-      <c r="X13" s="12"/>
-      <c r="Y13" s="12"/>
-      <c r="Z13" s="13"/>
-    </row>
-    <row r="14" spans="2:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E14">
-        <v>5</v>
-      </c>
-      <c r="F14" s="11"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
-      <c r="K14" s="2"/>
-      <c r="L14" s="2"/>
-      <c r="M14" s="2"/>
-      <c r="N14" s="2"/>
-      <c r="O14" s="2"/>
-      <c r="P14" s="2"/>
-      <c r="Q14" s="2"/>
-      <c r="R14" s="2"/>
-      <c r="S14" s="2"/>
-      <c r="T14" s="2"/>
-      <c r="U14" s="2"/>
-      <c r="V14" s="2"/>
-      <c r="W14" s="2"/>
-      <c r="X14" s="12"/>
-      <c r="Y14" s="12"/>
-      <c r="Z14" s="13"/>
-    </row>
-    <row r="15" spans="2:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E15">
-        <v>5</v>
-      </c>
-      <c r="F15" s="6"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
-      <c r="K15" s="2"/>
-      <c r="L15" s="2"/>
-      <c r="M15" s="2"/>
-      <c r="N15" s="2"/>
-      <c r="O15" s="2"/>
-      <c r="P15" s="2"/>
-      <c r="Q15" s="2"/>
-      <c r="R15" s="2"/>
-      <c r="S15" s="2"/>
-      <c r="T15" s="2"/>
-      <c r="U15" s="2"/>
-      <c r="V15" s="2"/>
-      <c r="W15" s="2"/>
-      <c r="X15" s="2"/>
-      <c r="Y15" s="2"/>
-      <c r="Z15" s="7"/>
-    </row>
-    <row r="16" spans="2:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E16">
-        <v>5</v>
-      </c>
-      <c r="F16" s="6"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
-      <c r="K16" s="2"/>
-      <c r="L16" s="2"/>
-      <c r="M16" s="2"/>
-      <c r="N16" s="2"/>
-      <c r="O16" s="2"/>
-      <c r="P16" s="2"/>
-      <c r="Q16" s="2"/>
-      <c r="R16" s="2"/>
-      <c r="S16" s="2"/>
-      <c r="T16" s="2"/>
-      <c r="U16" s="2"/>
-      <c r="V16" s="2"/>
-      <c r="W16" s="2"/>
-      <c r="X16" s="2"/>
-      <c r="Y16" s="2"/>
-      <c r="Z16" s="7"/>
-    </row>
-    <row r="17" spans="5:26" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E17">
-        <v>5</v>
-      </c>
-      <c r="F17" s="8"/>
-      <c r="G17" s="9"/>
-      <c r="H17" s="9"/>
-      <c r="I17" s="9"/>
-      <c r="J17" s="9"/>
-      <c r="K17" s="9"/>
-      <c r="L17" s="9"/>
-      <c r="M17" s="9"/>
-      <c r="N17" s="9"/>
-      <c r="O17" s="9"/>
-      <c r="P17" s="9"/>
-      <c r="Q17" s="9"/>
-      <c r="R17" s="9"/>
-      <c r="S17" s="9"/>
-      <c r="T17" s="9"/>
-      <c r="U17" s="9"/>
-      <c r="V17" s="9"/>
-      <c r="W17" s="9"/>
-      <c r="X17" s="9"/>
-      <c r="Y17" s="9"/>
-      <c r="Z17" s="10"/>
-    </row>
-    <row r="18" spans="5:26" x14ac:dyDescent="0.25">
-      <c r="E18" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F18">
-        <v>5</v>
-      </c>
-      <c r="G18">
-        <v>5</v>
-      </c>
-      <c r="H18">
-        <v>5</v>
-      </c>
-      <c r="I18">
-        <v>5</v>
-      </c>
-      <c r="J18">
-        <v>5</v>
-      </c>
-      <c r="K18">
-        <v>5</v>
-      </c>
-      <c r="L18">
-        <v>5</v>
-      </c>
-      <c r="M18">
-        <v>5</v>
-      </c>
-      <c r="N18">
-        <v>5</v>
-      </c>
-      <c r="O18">
-        <v>5</v>
-      </c>
-      <c r="P18">
-        <v>5</v>
-      </c>
-      <c r="Q18">
-        <v>5</v>
-      </c>
-      <c r="R18">
-        <v>5</v>
-      </c>
-      <c r="S18">
-        <v>5</v>
-      </c>
-      <c r="T18">
-        <v>5</v>
-      </c>
-      <c r="U18">
-        <v>5</v>
-      </c>
-      <c r="V18">
-        <v>5</v>
-      </c>
-      <c r="W18">
-        <v>5</v>
-      </c>
-      <c r="X18">
-        <v>5</v>
-      </c>
-      <c r="Y18">
-        <v>5</v>
-      </c>
-      <c r="Z18">
-        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -1815,10 +1837,10 @@
       <c r="B2" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="18" t="s">
+      <c r="C2" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="D2" s="18">
+      <c r="D2" s="17">
         <v>0</v>
       </c>
     </row>
@@ -1829,10 +1851,10 @@
       <c r="B3" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="D3" s="18">
+      <c r="D3" s="17">
         <v>0</v>
       </c>
     </row>
@@ -1843,10 +1865,10 @@
       <c r="B4" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="18" t="s">
+      <c r="C4" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="D4" s="18">
+      <c r="D4" s="17">
         <v>0</v>
       </c>
     </row>
@@ -1857,10 +1879,10 @@
       <c r="B5" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="18" t="s">
+      <c r="C5" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="D5" s="18">
+      <c r="D5" s="17">
         <v>0</v>
       </c>
     </row>
@@ -1874,7 +1896,7 @@
       <c r="C6" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="19">
+      <c r="D6" s="18">
         <v>0</v>
       </c>
     </row>
@@ -1888,7 +1910,7 @@
       <c r="C7" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="19">
+      <c r="D7" s="18">
         <v>0</v>
       </c>
     </row>
@@ -1899,7 +1921,7 @@
       <c r="B8" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="18" t="s">
+      <c r="C8" s="17" t="s">
         <v>30</v>
       </c>
       <c r="D8" t="s">
@@ -1937,7 +1959,7 @@
       <c r="B9" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="18" t="s">
+      <c r="C9" s="17" t="s">
         <v>44</v>
       </c>
       <c r="D9" t="s">
@@ -1951,7 +1973,7 @@
       <c r="B10" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="18" t="s">
+      <c r="C10" s="17" t="s">
         <v>44</v>
       </c>
       <c r="D10" t="s">
@@ -1965,7 +1987,7 @@
       <c r="B11" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="18" t="s">
+      <c r="C11" s="17" t="s">
         <v>31</v>
       </c>
       <c r="D11" t="s">
@@ -1979,7 +2001,7 @@
       <c r="B12" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="18" t="s">
+      <c r="C12" s="17" t="s">
         <v>31</v>
       </c>
       <c r="D12" t="s">
@@ -1993,7 +2015,7 @@
       <c r="B13" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="18" t="s">
+      <c r="C13" s="17" t="s">
         <v>30</v>
       </c>
       <c r="D13" t="s">

</xml_diff>